<commit_message>
[src/anonimization.py] Rewrite anonymization_coords function
</commit_message>
<xml_diff>
--- a/output/example.xlsx
+++ b/output/example.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>30.49,59.75</t>
+          <t>Колпинский район</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30.32,59.87</t>
+          <t>Московский район</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>30.38,60.09</t>
+          <t>Всеволожский район (Ленинградская область)</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>30.34,60.06</t>
+          <t>Выборгский район</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>30.42,59.85</t>
+          <t>Фрунзенский район</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30.35,60.07</t>
+          <t>Выборгский район</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>30.42,59.94</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>30.42,59.94</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>30.38,60.09</t>
+          <t>Всеволожский район (Ленинградская область)</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>30.23,59.98</t>
+          <t>Приморский район</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>30.42,59.83</t>
+          <t>Фрунзенский район</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>30.42,59.94</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>30.47,59.92</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>30.35,59.91</t>
+          <t>Фрунзенский район</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>30.42,59.94</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>30.48,59.91</t>
+          <t>Невский район</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>30.34,60.06</t>
+          <t>Выборгский район</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>30.38,60.09</t>
+          <t>Всеволожский район (Ленинградская область)</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>30.30,59.91</t>
+          <t>Адмиралтейский район</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>30.42,59.94</t>
+          <t>Красногвардейский район</t>
         </is>
       </c>
     </row>
@@ -765,43 +765,31 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>30.26,60.00</t>
+          <t>Приморский район</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Лента</t>
+          <t>О'КЕЙ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>30.33,59.90</t>
+          <t>Московский район</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>О'КЕЙ</t>
+          <t>Спортмастер</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>30.31,59.88</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Спортмастер</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>30.36,59.93</t>
+          <t>Центральный район</t>
         </is>
       </c>
     </row>

</xml_diff>